<commit_message>
Added code for wrangling
Motor vehicle census difference
</commit_message>
<xml_diff>
--- a/MotorVehicleCensus/By year.xlsx
+++ b/MotorVehicleCensus/By year.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harold_l/Downloads/MotorVehicleCensus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harold_l/Documents/GitHub/COMP20008-Project2/MotorVehicleCensus/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B4049E-E1F9-E74E-AD49-FCCB524B4672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D6D552-5671-EF4F-9B32-E1AD1466C7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="18420" xr2:uid="{792F2696-0F39-0440-92B1-D565624B91A6}"/>
   </bookViews>
@@ -73,9 +73,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="167" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -128,13 +127,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -455,15 +451,16 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="8" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -502,7 +499,7 @@
       <c r="C2" s="1">
         <v>3581815</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="2">
         <v>3666505</v>
       </c>
       <c r="E2" s="2">
@@ -528,7 +525,7 @@
       <c r="C3" s="1">
         <v>12687</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <v>13118</v>
       </c>
       <c r="E3" s="2">

</xml_diff>